<commit_message>
feat: handle invalid data
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t xml:space="preserve">TEL CLIENT</t>
   </si>
@@ -37,16 +37,16 @@
     <t xml:space="preserve">+212661250473</t>
   </si>
   <si>
-    <t xml:space="preserve">'+212 *6 5/4 -05= 02 9</t>
+    <t xml:space="preserve">+212611250473</t>
   </si>
   <si>
-    <t xml:space="preserve">661772696</t>
+    <t xml:space="preserve">+21261125047</t>
   </si>
   <si>
-    <t xml:space="preserve">00212661250473</t>
+    <t xml:space="preserve">+2122323</t>
   </si>
   <si>
-    <t xml:space="preserve">0021266125473</t>
+    <t xml:space="preserve">+2126111111111</t>
   </si>
 </sst>
 </file>
@@ -162,12 +162,12 @@
   <dimension ref="A1:C115"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -205,7 +205,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>3128871</v>
@@ -216,39 +216,41 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>2894456</v>
+        <v>123</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>15370.78</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="2" t="n">
-        <v>3174224</v>
+        <v>234</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>18414.38</v>
+        <v>234</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>234</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="2" t="n">
-        <v>3174224</v>
-      </c>
-      <c r="C7" s="2" t="n">
-        <v>18414.38</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
     </row>

</xml_diff>